<commit_message>
New list with coordinates
</commit_message>
<xml_diff>
--- a/list_of_station_and_range/Combined_Metadata.xlsx
+++ b/list_of_station_and_range/Combined_Metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\nishma\list_of_station_and_range\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1.Python\code_learning\list_of_station_and_range\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA45FF73-3E32-4207-8393-3C111BA38E02}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAE4609-54C3-4C70-A08D-D74592AC92B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8304" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1307,6 +1307,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1654,13 +1655,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I317"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A237" workbookViewId="0">
-      <selection activeCell="P282" sqref="P282"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F230" sqref="F230"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1689,7 +1700,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1718,7 +1729,7 @@
         <v>27.915126625598909</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1747,7 +1758,7 @@
         <v>40.090349075975361</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1776,7 +1787,7 @@
         <v>36.668035592060242</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1805,7 +1816,7 @@
         <v>56.336755646817252</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1834,7 +1845,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1863,7 +1874,7 @@
         <v>14.91581108829569</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1892,7 +1903,7 @@
         <v>16.167008898015059</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1921,7 +1932,7 @@
         <v>60.585900068446271</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1950,7 +1961,7 @@
         <v>60.829568788501028</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1979,7 +1990,7 @@
         <v>12.58590006844627</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2008,7 +2019,7 @@
         <v>57.585215605749489</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -2037,7 +2048,7 @@
         <v>12.336755646817251</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -2066,7 +2077,7 @@
         <v>14.160164271047231</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -2095,7 +2106,7 @@
         <v>14.160164271047231</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -2124,7 +2135,7 @@
         <v>13.831622176591379</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -2153,7 +2164,7 @@
         <v>48.495550992470911</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -2182,7 +2193,7 @@
         <v>43.080082135523611</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -2211,7 +2222,7 @@
         <v>40.249144421629019</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -2240,7 +2251,7 @@
         <v>36.249144421629019</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -2269,7 +2280,7 @@
         <v>51.586584531143053</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -2298,7 +2309,7 @@
         <v>52.334017796030118</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -2327,7 +2338,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -2356,7 +2367,7 @@
         <v>24.19986310746064</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -2385,7 +2396,7 @@
         <v>42.499657768651609</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -2414,7 +2425,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -2443,7 +2454,7 @@
         <v>26.165639972621491</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -2472,7 +2483,7 @@
         <v>20.123203285420949</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -2501,7 +2512,7 @@
         <v>15.7864476386037</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -2530,7 +2541,7 @@
         <v>24.161533196440789</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -2559,7 +2570,7 @@
         <v>18.083504449007531</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -2588,7 +2599,7 @@
         <v>12.49828884325804</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -2617,7 +2628,7 @@
         <v>15.337440109514031</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -2646,7 +2657,7 @@
         <v>18.083504449007531</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -2675,7 +2686,7 @@
         <v>15.249828884325799</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -2704,7 +2715,7 @@
         <v>12.25188227241615</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -2733,7 +2744,7 @@
         <v>12.91444216290212</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -2762,7 +2773,7 @@
         <v>13.16632443531828</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -2791,7 +2802,7 @@
         <v>13.33333333333333</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -2820,7 +2831,7 @@
         <v>11.50171115674196</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -2849,7 +2860,7 @@
         <v>11.91512662559891</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -2878,7 +2889,7 @@
         <v>12.249144421629021</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -2907,7 +2918,7 @@
         <v>10.67214236824093</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>9</v>
       </c>
@@ -2936,7 +2947,7 @@
         <v>10.53798767967146</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>74</v>
       </c>
@@ -2965,7 +2976,7 @@
         <v>56.555783709787818</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>74</v>
       </c>
@@ -2994,7 +3005,7 @@
         <v>25.66735112936345</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>74</v>
       </c>
@@ -3023,7 +3034,7 @@
         <v>57.4154688569473</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>80</v>
       </c>
@@ -3052,7 +3063,7 @@
         <v>29.916495550992469</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>80</v>
       </c>
@@ -3081,7 +3092,7 @@
         <v>46.75427789185489</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>80</v>
       </c>
@@ -3110,7 +3121,7 @@
         <v>26.91581108829569</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>80</v>
       </c>
@@ -3139,7 +3150,7 @@
         <v>15.91512662559891</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>80</v>
       </c>
@@ -3168,7 +3179,7 @@
         <v>19.74811772758385</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>80</v>
       </c>
@@ -3197,7 +3208,7 @@
         <v>20.668035592060232</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>80</v>
       </c>
@@ -3226,7 +3237,7 @@
         <v>20.668035592060232</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>80</v>
       </c>
@@ -3255,7 +3266,7 @@
         <v>22.50239561943874</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>80</v>
       </c>
@@ -3284,7 +3295,7 @@
         <v>16.585900068446271</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>80</v>
       </c>
@@ -3313,7 +3324,7 @@
         <v>14.25051334702259</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>80</v>
       </c>
@@ -3342,7 +3353,7 @@
         <v>14.25051334702259</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>80</v>
       </c>
@@ -3371,7 +3382,7 @@
         <v>14.25051334702259</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>80</v>
       </c>
@@ -3400,7 +3411,7 @@
         <v>14.33538672142368</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>80</v>
       </c>
@@ -3429,7 +3440,7 @@
         <v>14.25051334702259</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>80</v>
       </c>
@@ -3458,7 +3469,7 @@
         <v>13.33333333333333</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>80</v>
       </c>
@@ -3487,7 +3498,7 @@
         <v>13.66735112936345</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>80</v>
       </c>
@@ -3516,7 +3527,7 @@
         <v>10.16563997262149</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>105</v>
       </c>
@@ -3545,7 +3556,7 @@
         <v>10.74880219028063</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>105</v>
       </c>
@@ -3574,7 +3585,7 @@
         <v>61.913757700205338</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>105</v>
       </c>
@@ -3603,7 +3614,7 @@
         <v>15.75359342915811</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>105</v>
       </c>
@@ -3632,7 +3643,7 @@
         <v>26.91581108829569</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>105</v>
       </c>
@@ -3661,7 +3672,7 @@
         <v>18.751540041067759</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>105</v>
       </c>
@@ -3690,7 +3701,7 @@
         <v>11.167693360711841</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>105</v>
       </c>
@@ -3719,7 +3730,7 @@
         <v>17.828884325804239</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>105</v>
       </c>
@@ -3748,7 +3759,7 @@
         <v>17.33607118412047</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>105</v>
       </c>
@@ -3777,7 +3788,7 @@
         <v>13.96030116358658</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>105</v>
       </c>
@@ -3806,7 +3817,7 @@
         <v>12.49828884325804</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>105</v>
       </c>
@@ -3835,7 +3846,7 @@
         <v>18.335386721423681</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>105</v>
       </c>
@@ -3864,7 +3875,7 @@
         <v>13.66735112936345</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>105</v>
       </c>
@@ -3893,7 +3904,7 @@
         <v>11.832991101984939</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>105</v>
       </c>
@@ -3922,7 +3933,7 @@
         <v>12.32854209445585</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>105</v>
       </c>
@@ -3951,7 +3962,7 @@
         <v>12.334017796030119</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>105</v>
       </c>
@@ -3980,7 +3991,7 @@
         <v>15.07734428473648</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>105</v>
       </c>
@@ -4009,7 +4020,7 @@
         <v>22.91581108829569</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>105</v>
       </c>
@@ -4038,7 +4049,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>128</v>
       </c>
@@ -4067,7 +4078,7 @@
         <v>25.998631074606429</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>128</v>
       </c>
@@ -4096,7 +4107,7 @@
         <v>40.45722108145106</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>128</v>
       </c>
@@ -4125,7 +4136,7 @@
         <v>12.35044490075291</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>128</v>
       </c>
@@ -4154,7 +4165,7 @@
         <v>37.081451060917182</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>128</v>
       </c>
@@ -4183,7 +4194,7 @@
         <v>29.081451060917178</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>128</v>
       </c>
@@ -4212,7 +4223,7 @@
         <v>34.918548939082818</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>128</v>
       </c>
@@ -4241,7 +4252,7 @@
         <v>52.999315537303218</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>128</v>
       </c>
@@ -4270,7 +4281,7 @@
         <v>26.075290896646131</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>128</v>
       </c>
@@ -4299,7 +4310,7 @@
         <v>27.665982203969879</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>128</v>
       </c>
@@ -4328,7 +4339,7 @@
         <v>56.91444216290212</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>128</v>
       </c>
@@ -4357,7 +4368,7 @@
         <v>14.083504449007529</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>128</v>
       </c>
@@ -4386,7 +4397,7 @@
         <v>46.168377823408633</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>128</v>
       </c>
@@ -4415,7 +4426,7 @@
         <v>16.25188227241615</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>128</v>
       </c>
@@ -4444,7 +4455,7 @@
         <v>10.50239561943874</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>128</v>
       </c>
@@ -4473,7 +4484,7 @@
         <v>41.664613278576319</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>128</v>
       </c>
@@ -4502,7 +4513,7 @@
         <v>24.832306639288159</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>128</v>
       </c>
@@ -4531,7 +4542,7 @@
         <v>13.24572210814511</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>128</v>
       </c>
@@ -4560,7 +4571,7 @@
         <v>13.24572210814511</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>128</v>
       </c>
@@ -4589,7 +4600,7 @@
         <v>12.99931553730322</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>128</v>
       </c>
@@ -4618,7 +4629,7 @@
         <v>30.247775496235459</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>128</v>
       </c>
@@ -4647,7 +4658,7 @@
         <v>12.75290896646133</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>128</v>
       </c>
@@ -4676,7 +4687,7 @@
         <v>11.504449007529089</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>159</v>
       </c>
@@ -4705,7 +4716,7 @@
         <v>11.329226557152641</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>159</v>
       </c>
@@ -4734,7 +4745,7 @@
         <v>49.503080082135533</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>159</v>
       </c>
@@ -4763,7 +4774,7 @@
         <v>27.75633127994524</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>159</v>
       </c>
@@ -4792,7 +4803,7 @@
         <v>14.91581108829569</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>159</v>
       </c>
@@ -4821,7 +4832,7 @@
         <v>14.91581108829569</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>159</v>
       </c>
@@ -4850,7 +4861,7 @@
         <v>12.580424366872011</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>159</v>
       </c>
@@ -4879,7 +4890,7 @@
         <v>14.91581108829569</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>159</v>
       </c>
@@ -4908,7 +4919,7 @@
         <v>17.746748802190279</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>159</v>
       </c>
@@ -4937,7 +4948,7 @@
         <v>11.41409993155373</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>159</v>
       </c>
@@ -4966,7 +4977,7 @@
         <v>10.499657768651611</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>159</v>
       </c>
@@ -4995,7 +5006,7 @@
         <v>49.075975359342912</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>159</v>
       </c>
@@ -5024,7 +5035,7 @@
         <v>19.915126625598909</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>159</v>
       </c>
@@ -5053,7 +5064,7 @@
         <v>37.828884325804253</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>159</v>
       </c>
@@ -5082,7 +5093,7 @@
         <v>13.746748802190281</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>159</v>
       </c>
@@ -5111,7 +5122,7 @@
         <v>13.585215605749489</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>159</v>
       </c>
@@ -5140,7 +5151,7 @@
         <v>13.746748802190281</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>159</v>
       </c>
@@ -5169,7 +5180,7 @@
         <v>13.746748802190281</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>159</v>
       </c>
@@ -5198,7 +5209,7 @@
         <v>13.746748802190281</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>159</v>
       </c>
@@ -5227,7 +5238,7 @@
         <v>13.08418891170431</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>185</v>
       </c>
@@ -5256,7 +5267,7 @@
         <v>54.417522245037652</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>185</v>
       </c>
@@ -5285,7 +5296,7 @@
         <v>29.494866529774129</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>185</v>
       </c>
@@ -5314,7 +5325,7 @@
         <v>15.24709103353867</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>185</v>
       </c>
@@ -5343,7 +5354,7 @@
         <v>14.83093771389459</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>185</v>
       </c>
@@ -5372,7 +5383,7 @@
         <v>14.91581108829569</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>185</v>
       </c>
@@ -5401,7 +5412,7 @@
         <v>14.91854893908282</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>185</v>
       </c>
@@ -5430,7 +5441,7 @@
         <v>12.58590006844627</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>185</v>
       </c>
@@ -5459,7 +5470,7 @@
         <v>29.16632443531828</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>185</v>
       </c>
@@ -5488,7 +5499,7 @@
         <v>38.0807665982204</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>185</v>
       </c>
@@ -5517,7 +5528,7 @@
         <v>13.913757700205339</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>185</v>
       </c>
@@ -5546,7 +5557,7 @@
         <v>52.91444216290212</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>185</v>
       </c>
@@ -5575,7 +5586,7 @@
         <v>52.91444216290212</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>185</v>
       </c>
@@ -5604,7 +5615,7 @@
         <v>52.91444216290212</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>185</v>
       </c>
@@ -5633,7 +5644,7 @@
         <v>52.747433264887057</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>185</v>
       </c>
@@ -5662,7 +5673,7 @@
         <v>52.91444216290212</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>185</v>
       </c>
@@ -5691,7 +5702,7 @@
         <v>52.91444216290212</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>185</v>
       </c>
@@ -5720,7 +5731,7 @@
         <v>35.249828884325801</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>185</v>
       </c>
@@ -5749,7 +5760,7 @@
         <v>35.915126625598901</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>185</v>
       </c>
@@ -5778,7 +5789,7 @@
         <v>30.327173169062281</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>185</v>
       </c>
@@ -5807,7 +5818,7 @@
         <v>11.750855578370979</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>185</v>
       </c>
@@ -5836,7 +5847,7 @@
         <v>41.667351129363453</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>185</v>
       </c>
@@ -5865,7 +5876,7 @@
         <v>40.585900068446271</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>185</v>
       </c>
@@ -5894,7 +5905,7 @@
         <v>27.58658453114305</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>185</v>
       </c>
@@ -5923,7 +5934,7 @@
         <v>25.831622176591381</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>185</v>
       </c>
@@ -5952,7 +5963,7 @@
         <v>28.91444216290212</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>185</v>
       </c>
@@ -5981,7 +5992,7 @@
         <v>19.753593429158109</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>185</v>
       </c>
@@ -6010,7 +6021,7 @@
         <v>13.629021218343601</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>218</v>
       </c>
@@ -6039,7 +6050,7 @@
         <v>13.831622176591379</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>218</v>
       </c>
@@ -6068,7 +6079,7 @@
         <v>16.495550992470911</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>218</v>
       </c>
@@ -6097,7 +6108,7 @@
         <v>43.082819986310753</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>218</v>
       </c>
@@ -6126,7 +6137,7 @@
         <v>62.751540041067763</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>218</v>
       </c>
@@ -6155,7 +6166,7 @@
         <v>61.667351129363453</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>218</v>
       </c>
@@ -6184,7 +6195,7 @@
         <v>13.57973990417522</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>218</v>
       </c>
@@ -6213,7 +6224,7 @@
         <v>30.50239561943874</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>218</v>
       </c>
@@ -6242,7 +6253,7 @@
         <v>21.672826830937719</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>218</v>
       </c>
@@ -6271,7 +6282,7 @@
         <v>21.451060917180008</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>218</v>
       </c>
@@ -6300,7 +6311,7 @@
         <v>28.947296372347711</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>218</v>
       </c>
@@ -6329,7 +6340,7 @@
         <v>48.752908966461327</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>218</v>
       </c>
@@ -6358,7 +6369,7 @@
         <v>21.43189596167009</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>218</v>
       </c>
@@ -6387,7 +6398,7 @@
         <v>28.947296372347711</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>218</v>
       </c>
@@ -6416,7 +6427,7 @@
         <v>42.91581108829569</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>218</v>
       </c>
@@ -6445,7 +6456,7 @@
         <v>52.334017796030118</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>218</v>
       </c>
@@ -6474,7 +6485,7 @@
         <v>52.334017796030118</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>218</v>
       </c>
@@ -6503,7 +6514,7 @@
         <v>53.333333333333343</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>218</v>
       </c>
@@ -6532,7 +6543,7 @@
         <v>51.247091033538673</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>218</v>
       </c>
@@ -6561,7 +6572,7 @@
         <v>18.751540041067759</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>218</v>
       </c>
@@ -6590,7 +6601,7 @@
         <v>58.502395619438737</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>218</v>
       </c>
@@ -6619,7 +6630,7 @@
         <v>24.668035592060232</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>218</v>
       </c>
@@ -6648,7 +6659,7 @@
         <v>23.419575633127991</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>218</v>
       </c>
@@ -6677,7 +6688,7 @@
         <v>35.83025325119781</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>218</v>
       </c>
@@ -6706,7 +6717,7 @@
         <v>61.166324435318273</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>218</v>
       </c>
@@ -6735,7 +6746,7 @@
         <v>59.83025325119781</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>218</v>
       </c>
@@ -6764,7 +6775,7 @@
         <v>16.501026694045169</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>218</v>
       </c>
@@ -6793,7 +6804,7 @@
         <v>29.08418891170431</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>218</v>
       </c>
@@ -6822,7 +6833,7 @@
         <v>22.168377823408619</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>218</v>
       </c>
@@ -6851,7 +6862,7 @@
         <v>16.585900068446271</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>218</v>
       </c>
@@ -6880,7 +6891,7 @@
         <v>16.585900068446271</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>218</v>
       </c>
@@ -6909,7 +6920,7 @@
         <v>27.915126625598909</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>218</v>
       </c>
@@ -6938,7 +6949,7 @@
         <v>13.916495550992471</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>218</v>
       </c>
@@ -6967,7 +6978,7 @@
         <v>22.91581108829569</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>218</v>
       </c>
@@ -6996,7 +7007,7 @@
         <v>61.828884325804253</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>218</v>
       </c>
@@ -7025,7 +7036,7 @@
         <v>40.167008898015062</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>218</v>
       </c>
@@ -7054,7 +7065,7 @@
         <v>14.581793292265569</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>218</v>
       </c>
@@ -7083,7 +7094,7 @@
         <v>15.16495550992471</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>218</v>
       </c>
@@ -7112,7 +7123,7 @@
         <v>10.757015742642031</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>218</v>
       </c>
@@ -7141,7 +7152,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>218</v>
       </c>
@@ -7170,7 +7181,7 @@
         <v>59.419575633127998</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>218</v>
       </c>
@@ -7199,7 +7210,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>218</v>
       </c>
@@ -7228,7 +7239,7 @@
         <v>59.586584531143053</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>218</v>
       </c>
@@ -7257,7 +7268,7 @@
         <v>58.751540041067763</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>218</v>
       </c>
@@ -7286,7 +7297,7 @@
         <v>57.752224503764538</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>218</v>
       </c>
@@ -7315,7 +7326,7 @@
         <v>13.585215605749489</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>218</v>
       </c>
@@ -7344,7 +7355,7 @@
         <v>17.913757700205341</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>218</v>
       </c>
@@ -7373,7 +7384,7 @@
         <v>22.165639972621491</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>218</v>
       </c>
@@ -7402,7 +7413,7 @@
         <v>22.165639972621491</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>218</v>
       </c>
@@ -7431,7 +7442,7 @@
         <v>11.91512662559891</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>218</v>
       </c>
@@ -7460,7 +7471,7 @@
         <v>21.670088980150581</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>218</v>
       </c>
@@ -7489,7 +7500,7 @@
         <v>17.007529089664612</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>218</v>
       </c>
@@ -7518,7 +7529,7 @@
         <v>16.917180013689251</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>218</v>
       </c>
@@ -7547,7 +7558,7 @@
         <v>16.917180013689251</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>218</v>
       </c>
@@ -7576,7 +7587,7 @@
         <v>14.329911019849421</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>218</v>
       </c>
@@ -7605,7 +7616,7 @@
         <v>19.080082135523611</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>218</v>
       </c>
@@ -7634,7 +7645,7 @@
         <v>17.831622176591381</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>218</v>
       </c>
@@ -7663,7 +7674,7 @@
         <v>13.913757700205339</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>218</v>
       </c>
@@ -7692,7 +7703,7 @@
         <v>13.913757700205339</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>218</v>
       </c>
@@ -7721,7 +7732,7 @@
         <v>32.91444216290212</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>218</v>
       </c>
@@ -7750,7 +7761,7 @@
         <v>33.913757700205338</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>218</v>
       </c>
@@ -7779,7 +7790,7 @@
         <v>34.91581108829569</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>218</v>
       </c>
@@ -7808,7 +7819,7 @@
         <v>34.91581108829569</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>218</v>
       </c>
@@ -7837,7 +7848,7 @@
         <v>34.91581108829569</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>218</v>
       </c>
@@ -7866,7 +7877,7 @@
         <v>34.338124572210823</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>218</v>
       </c>
@@ -7895,7 +7906,7 @@
         <v>35.915126625598901</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>218</v>
       </c>
@@ -7924,7 +7935,7 @@
         <v>30.91581108829569</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>218</v>
       </c>
@@ -7953,7 +7964,7 @@
         <v>32.91444216290212</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>218</v>
       </c>
@@ -7982,7 +7993,7 @@
         <v>35.915126625598901</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>218</v>
       </c>
@@ -8011,7 +8022,7 @@
         <v>35.915126625598901</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>218</v>
       </c>
@@ -8040,7 +8051,7 @@
         <v>35.915126625598901</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>218</v>
       </c>
@@ -8069,7 +8080,7 @@
         <v>35.915126625598901</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>218</v>
       </c>
@@ -8098,7 +8109,7 @@
         <v>25.916495550992469</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>218</v>
       </c>
@@ -8127,7 +8138,7 @@
         <v>35.915126625598901</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>218</v>
       </c>
@@ -8156,7 +8167,7 @@
         <v>21.752224503764541</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>218</v>
       </c>
@@ -8185,7 +8196,7 @@
         <v>21.670088980150581</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>218</v>
       </c>
@@ -8214,7 +8225,7 @@
         <v>21.831622176591381</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>218</v>
       </c>
@@ -8243,7 +8254,7 @@
         <v>21.831622176591381</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>218</v>
       </c>
@@ -8272,7 +8283,7 @@
         <v>21.831622176591381</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>218</v>
       </c>
@@ -8301,7 +8312,7 @@
         <v>21.831622176591381</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>218</v>
       </c>
@@ -8330,7 +8341,7 @@
         <v>21.752224503764541</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>218</v>
       </c>
@@ -8359,7 +8370,7 @@
         <v>21.752224503764541</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>218</v>
       </c>
@@ -8388,7 +8399,7 @@
         <v>21.831622176591381</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>218</v>
       </c>
@@ -8417,7 +8428,7 @@
         <v>21.831622176591381</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>218</v>
       </c>
@@ -8446,7 +8457,7 @@
         <v>21.752224503764541</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>218</v>
       </c>
@@ -8475,7 +8486,7 @@
         <v>21.916495550992469</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>218</v>
       </c>
@@ -8504,7 +8515,7 @@
         <v>21.752224503764541</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>218</v>
       </c>
@@ -8533,7 +8544,7 @@
         <v>21.585215605749489</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>218</v>
       </c>
@@ -8562,7 +8573,7 @@
         <v>21.831622176591381</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>218</v>
       </c>
@@ -8591,7 +8602,7 @@
         <v>15.83025325119781</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>218</v>
       </c>
@@ -8620,7 +8631,7 @@
         <v>32.752908966461327</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>218</v>
       </c>
@@ -8649,7 +8660,7 @@
         <v>52.829568788501028</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>218</v>
       </c>
@@ -8678,7 +8689,7 @@
         <v>14.417522245037651</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>218</v>
       </c>
@@ -8707,7 +8718,7 @@
         <v>14.417522245037651</v>
       </c>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>218</v>
       </c>
@@ -8736,7 +8747,7 @@
         <v>14.247775496235461</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>218</v>
       </c>
@@ -8765,7 +8776,7 @@
         <v>14.417522245037651</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>218</v>
       </c>
@@ -8794,7 +8805,7 @@
         <v>29.913757700205341</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>218</v>
       </c>
@@ -8823,7 +8834,7 @@
         <v>29.913757700205341</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>218</v>
       </c>
@@ -8852,7 +8863,7 @@
         <v>29.913757700205341</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>218</v>
       </c>
@@ -8881,7 +8892,7 @@
         <v>29.913757700205341</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>218</v>
       </c>
@@ -8910,7 +8921,7 @@
         <v>18.91581108829569</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>218</v>
       </c>
@@ -8939,7 +8950,7 @@
         <v>19.915126625598909</v>
       </c>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>218</v>
       </c>
@@ -8968,7 +8979,7 @@
         <v>28.418891170431209</v>
       </c>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>218</v>
       </c>
@@ -8997,7 +9008,7 @@
         <v>31.41683778234086</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>218</v>
       </c>
@@ -9026,7 +9037,7 @@
         <v>27.665982203969879</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>218</v>
       </c>
@@ -9055,7 +9066,7 @@
         <v>23.337440109514031</v>
       </c>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>218</v>
       </c>
@@ -9084,7 +9095,7 @@
         <v>11.83025325119781</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>218</v>
       </c>
@@ -9113,7 +9124,7 @@
         <v>11.24709103353867</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>218</v>
       </c>
@@ -9142,7 +9153,7 @@
         <v>11.082819986310749</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>218</v>
       </c>
@@ -9171,7 +9182,7 @@
         <v>12.501026694045169</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>218</v>
       </c>
@@ -9200,7 +9211,7 @@
         <v>16.501026694045169</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>218</v>
       </c>
@@ -9229,7 +9240,7 @@
         <v>12.99931553730322</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>218</v>
       </c>
@@ -9258,7 +9269,7 @@
         <v>16.501026694045169</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>218</v>
       </c>
@@ -9287,7 +9298,7 @@
         <v>11.419575633127989</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>218</v>
       </c>
@@ -9316,7 +9327,7 @@
         <v>16.418891170431209</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>218</v>
       </c>
@@ -9345,7 +9356,7 @@
         <v>16.501026694045169</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>218</v>
       </c>
@@ -9374,7 +9385,7 @@
         <v>16.501026694045169</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>218</v>
       </c>
@@ -9403,7 +9414,7 @@
         <v>16.501026694045169</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>218</v>
       </c>
@@ -9432,7 +9443,7 @@
         <v>16.501026694045169</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>361</v>
       </c>
@@ -9461,7 +9472,7 @@
         <v>26.42026009582478</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>361</v>
       </c>
@@ -9490,7 +9501,7 @@
         <v>26.669404517453799</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>361</v>
       </c>
@@ -9519,7 +9530,7 @@
         <v>10.33538672142368</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>361</v>
       </c>
@@ -9548,7 +9559,7 @@
         <v>16.084873374401091</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>361</v>
       </c>
@@ -9577,7 +9588,7 @@
         <v>11.329226557152641</v>
       </c>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>361</v>
       </c>
@@ -9606,7 +9617,7 @@
         <v>31.419575633127991</v>
       </c>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>361</v>
       </c>
@@ -9635,7 +9646,7 @@
         <v>14.50239561943874</v>
       </c>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>361</v>
       </c>
@@ -9664,7 +9675,7 @@
         <v>29.251197809719368</v>
       </c>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>361</v>
       </c>
@@ -9693,7 +9704,7 @@
         <v>31.663244353182751</v>
       </c>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>361</v>
       </c>
@@ -9722,7 +9733,7 @@
         <v>18.42026009582478</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>361</v>
       </c>
@@ -9751,7 +9762,7 @@
         <v>50.335386721423681</v>
       </c>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>361</v>
       </c>
@@ -9780,7 +9791,7 @@
         <v>14.25051334702259</v>
       </c>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>361</v>
       </c>
@@ -9809,7 +9820,7 @@
         <v>13.25119780971937</v>
       </c>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>361</v>
       </c>
@@ -9838,7 +9849,7 @@
         <v>28.454483230663929</v>
       </c>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>361</v>
       </c>
@@ -9867,7 +9878,7 @@
         <v>25.46201232032854</v>
       </c>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>361</v>
       </c>
@@ -9896,7 +9907,7 @@
         <v>24.832306639288159</v>
       </c>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>361</v>
       </c>
@@ -9925,7 +9936,7 @@
         <v>25.333333333333329</v>
       </c>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>361</v>
       </c>
@@ -9954,7 +9965,7 @@
         <v>20.999315537303222</v>
       </c>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>361</v>
       </c>
@@ -9983,7 +9994,7 @@
         <v>24.832306639288159</v>
       </c>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>361</v>
       </c>
@@ -10012,7 +10023,7 @@
         <v>22.409308692676252</v>
       </c>
     </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>361</v>
       </c>
@@ -10041,7 +10052,7 @@
         <v>28.454483230663929</v>
       </c>
     </row>
-    <row r="290" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>361</v>
       </c>
@@ -10070,7 +10081,7 @@
         <v>25.629021218343599</v>
       </c>
     </row>
-    <row r="291" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>361</v>
       </c>
@@ -10099,7 +10110,7 @@
         <v>25.831622176591381</v>
       </c>
     </row>
-    <row r="292" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>361</v>
       </c>
@@ -10128,7 +10139,7 @@
         <v>18.33264887063655</v>
       </c>
     </row>
-    <row r="293" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>361</v>
       </c>
@@ -10157,7 +10168,7 @@
         <v>13.33607118412047</v>
       </c>
     </row>
-    <row r="294" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>361</v>
       </c>
@@ -10186,7 +10197,7 @@
         <v>47.671457905544138</v>
       </c>
     </row>
-    <row r="295" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>361</v>
       </c>
@@ -10215,7 +10226,7 @@
         <v>11.249828884325799</v>
       </c>
     </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>361</v>
       </c>
@@ -10244,7 +10255,7 @@
         <v>21.081451060917178</v>
       </c>
     </row>
-    <row r="297" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>361</v>
       </c>
@@ -10273,7 +10284,7 @@
         <v>17.998631074606429</v>
       </c>
     </row>
-    <row r="298" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>361</v>
       </c>
@@ -10302,7 +10313,7 @@
         <v>39.663244353182748</v>
       </c>
     </row>
-    <row r="299" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>361</v>
       </c>
@@ -10331,7 +10342,7 @@
         <v>24.08213552361396</v>
       </c>
     </row>
-    <row r="300" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>361</v>
       </c>
@@ -10360,7 +10371,7 @@
         <v>24.498288843258042</v>
       </c>
     </row>
-    <row r="301" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>361</v>
       </c>
@@ -10389,7 +10400,7 @@
         <v>21.16632443531828</v>
       </c>
     </row>
-    <row r="302" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>361</v>
       </c>
@@ -10418,7 +10429,7 @@
         <v>15.082819986310749</v>
       </c>
     </row>
-    <row r="303" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>361</v>
       </c>
@@ -10447,7 +10458,7 @@
         <v>17.42368240930869</v>
       </c>
     </row>
-    <row r="304" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>361</v>
       </c>
@@ -10476,7 +10487,7 @@
         <v>17.790554414784399</v>
       </c>
     </row>
-    <row r="305" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>361</v>
       </c>
@@ -10505,7 +10516,7 @@
         <v>19.838466803559211</v>
       </c>
     </row>
-    <row r="306" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>361</v>
       </c>
@@ -10534,7 +10545,7 @@
         <v>20.75290896646133</v>
       </c>
     </row>
-    <row r="307" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>361</v>
       </c>
@@ -10563,7 +10574,7 @@
         <v>16.75290896646133</v>
       </c>
     </row>
-    <row r="308" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>361</v>
       </c>
@@ -10592,7 +10603,7 @@
         <v>13.16632443531828</v>
       </c>
     </row>
-    <row r="309" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>361</v>
       </c>
@@ -10621,7 +10632,7 @@
         <v>10.083504449007529</v>
       </c>
     </row>
-    <row r="310" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>361</v>
       </c>
@@ -10650,7 +10661,7 @@
         <v>52.249144421629019</v>
       </c>
     </row>
-    <row r="311" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>361</v>
       </c>
@@ -10679,7 +10690,7 @@
         <v>27.74811772758385</v>
       </c>
     </row>
-    <row r="312" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>361</v>
       </c>
@@ -10708,7 +10719,7 @@
         <v>28.91444216290212</v>
       </c>
     </row>
-    <row r="313" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>361</v>
       </c>
@@ -10737,7 +10748,7 @@
         <v>53.418206707734427</v>
       </c>
     </row>
-    <row r="314" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>361</v>
       </c>
@@ -10766,7 +10777,7 @@
         <v>27.504449007529089</v>
       </c>
     </row>
-    <row r="315" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>361</v>
       </c>
@@ -10795,7 +10806,7 @@
         <v>45.166324435318273</v>
       </c>
     </row>
-    <row r="316" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>361</v>
       </c>
@@ -10824,7 +10835,7 @@
         <v>15.167693360711841</v>
       </c>
     </row>
-    <row r="317" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>361</v>
       </c>

</xml_diff>